<commit_message>
Arbeitsaufzeichnung von Aron fertig
</commit_message>
<xml_diff>
--- a/Arbeitsaufzeichnungen/Arbeitsaufzeichnung_Aron.xlsx
+++ b/Arbeitsaufzeichnungen/Arbeitsaufzeichnung_Aron.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aronterzeta/Documents/Shkolla austriake 2019-2020/Diplom/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aronterzeta/Shkolla austriake/diplomarbeit/Arbeitsaufzeichnungen/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="92">
   <si>
     <t>Was</t>
   </si>
@@ -210,6 +210,99 @@
   </si>
   <si>
     <t xml:space="preserve">Prototyp verbessern (Admin nur Aron durch Vergleich zweien Bilder, Registrierung fertig) </t>
+  </si>
+  <si>
+    <t>Fehler in Log speichern</t>
+  </si>
+  <si>
+    <t>Status-Präsentation vorbereiten</t>
+  </si>
+  <si>
+    <t>13.12.2019-16.12.2019</t>
+  </si>
+  <si>
+    <t>23.12.2019-26.12.2019</t>
+  </si>
+  <si>
+    <t>Array der Gesichtspunkte in zwei aufteilen. Das erste ist nur für die x-Achse und das zweite für die y-Achse</t>
+  </si>
+  <si>
+    <t>04.01.2020-07.01.2020</t>
+  </si>
+  <si>
+    <t>1 Betreuertreffung</t>
+  </si>
+  <si>
+    <t>14.01.2020</t>
+  </si>
+  <si>
+    <t>Dokumentation Korrektur</t>
+  </si>
+  <si>
+    <t>17.01.2020</t>
+  </si>
+  <si>
+    <t>25.01.2020</t>
+  </si>
+  <si>
+    <t>3 Prototyps gemacht für Backups, wenn ein nicht funktioniert</t>
+  </si>
+  <si>
+    <t>25.01.2020-27-01.2020</t>
+  </si>
+  <si>
+    <t>Dokumentation verarbeiten, weiter mit der Korrektur, Struktur der Dokumentation verbessern</t>
+  </si>
+  <si>
+    <t>31.01.2020</t>
+  </si>
+  <si>
+    <t>In Registrierung-Teil arbeiten, verschiedene Skripts miteinander verbinden, die richtigen Konsole-Parameter von Skript zu Skript übergeben</t>
+  </si>
+  <si>
+    <t>01.02.2020-02.02.2020</t>
+  </si>
+  <si>
+    <t>Automatische Konfiguration von Opencv in Raspberry PI</t>
+  </si>
+  <si>
+    <t>03.02.2020</t>
+  </si>
+  <si>
+    <t>Log (in Datenbank und in einer Text-File)</t>
+  </si>
+  <si>
+    <t>05.02.2020</t>
+  </si>
+  <si>
+    <t>Anpassung des Registrierungsteils, weil in der DB etwas geändert hat (von zwei Tabellen, jetzt nur eine)</t>
+  </si>
+  <si>
+    <t>07.02.2020,08.02.2020</t>
+  </si>
+  <si>
+    <t>Das Problem mit dem Zugriff auf Elementen des numpy-Arrays analysieren und lösen</t>
+  </si>
+  <si>
+    <t>10.02.2020</t>
+  </si>
+  <si>
+    <t>11.02.2020-15.02.2020</t>
+  </si>
+  <si>
+    <t>Testen des Registrierungsteil</t>
+  </si>
+  <si>
+    <t>In der Finalabgabe der Dokumentation arbeiten</t>
+  </si>
+  <si>
+    <t>16.02.2020-20.02.2020, 30.02.2020-03.03.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die End-Präsentation von der Diplomarbeit </t>
+  </si>
+  <si>
+    <t>04.03.2020-06.03.2020</t>
   </si>
 </sst>
 </file>
@@ -241,9 +334,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -253,9 +355,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,15 +639,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="85" customWidth="1"/>
+    <col min="1" max="1" width="123.83203125" customWidth="1"/>
     <col min="2" max="2" width="61.33203125" customWidth="1"/>
     <col min="3" max="3" width="59.1640625" customWidth="1"/>
   </cols>
@@ -573,8 +679,8 @@
         <v>5</v>
       </c>
       <c r="E3">
-        <f>SUM(C3:C34)</f>
-        <v>101</v>
+        <f>SUM(C3:C50)</f>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -915,6 +1021,182 @@
         <v>58</v>
       </c>
       <c r="C34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C50">
         <v>5</v>
       </c>
     </row>

</xml_diff>